<commit_message>
Updated sprint 1 and architecture docs
</commit_message>
<xml_diff>
--- a/docs/P3 - Requirements Stack.xlsx
+++ b/docs/P3 - Requirements Stack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29421"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{934DD962-A46D-412A-9BC1-47F885305E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4325D8F-89E6-4069-96D0-264C42DA9017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -579,7 +579,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -689,7 +689,9 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1">
@@ -721,7 +723,9 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1">
@@ -736,7 +740,9 @@
       <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1">
@@ -751,7 +757,9 @@
       <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1">
@@ -811,7 +819,9 @@
       <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1">
@@ -826,7 +836,9 @@
       <c r="D15" s="1">
         <v>1</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1">
@@ -841,7 +853,9 @@
       <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="29.25">
       <c r="A17" s="1">
@@ -856,7 +870,9 @@
       <c r="D17" s="1">
         <v>1</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="29.25">
       <c r="A18" s="1">
@@ -871,7 +887,9 @@
       <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="29.25">
       <c r="A19" s="1">
@@ -886,7 +904,9 @@
       <c r="D19" s="1">
         <v>1</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1">
@@ -935,7 +955,9 @@
       <c r="D22" s="1">
         <v>1</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="29.25">
       <c r="A23" s="1">
@@ -950,7 +972,9 @@
       <c r="D23" s="1">
         <v>2</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="29.25">
       <c r="A24" s="1">
@@ -980,7 +1004,9 @@
       <c r="D25" s="1">
         <v>2</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="29.25">
       <c r="A26" s="1">
@@ -1100,7 +1126,9 @@
       <c r="D33" s="1">
         <v>4</v>
       </c>
-      <c r="E33" s="1"/>
+      <c r="E33" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1">
@@ -1115,7 +1143,9 @@
       <c r="D34" s="1">
         <v>4</v>
       </c>
-      <c r="E34" s="1"/>
+      <c r="E34" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1">
@@ -1130,7 +1160,9 @@
       <c r="D35" s="1">
         <v>4</v>
       </c>
-      <c r="E35" s="1"/>
+      <c r="E35" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1">
@@ -1216,8 +1248,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF0891E31D3F4748B96BA1AD6C8516D0" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c6ad350ae23677189d25aea62ebfdb06">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b3dee608-f3e3-4732-bac7-04ace8bc815d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="90ba9d69135dc0ff0aa81b0c153a4ef5" ns2:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF0891E31D3F4748B96BA1AD6C8516D0" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e6a7620b83dbdb6bccc61e22e4ed2fa">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b3dee608-f3e3-4732-bac7-04ace8bc815d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="25b88dee9cc6fe20bc8c4b3e1587c0f6" ns2:_="">
     <xsd:import namespace="b3dee608-f3e3-4732-bac7-04ace8bc815d"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -1353,12 +1391,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1369,11 +1401,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5E9C4BD-28F5-4DE7-AA91-CEAB833D2EC4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE7E8F8E-4E47-4472-B67A-83324F2DF2FE}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE7E8F8E-4E47-4472-B67A-83324F2DF2FE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3715750-B029-4E46-8D16-CBA6CFC4C418}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>